<commit_message>
GetDataFromExcel issue fixed for AddAsset Excel sheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/fnb/qa/testdata/FnB_AddAssetTestData.xlsx
+++ b/src/main/java/com/fnb/qa/testdata/FnB_AddAssetTestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
-    <sheet name="Contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="AddAsset" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>AssetNo</t>
   </si>
@@ -56,7 +56,37 @@
     <t>C1</t>
   </si>
   <si>
-    <t>Test Product</t>
+    <t>Test Product 1</t>
+  </si>
+  <si>
+    <t>AAA-5030543</t>
+  </si>
+  <si>
+    <t>MA-7383994</t>
+  </si>
+  <si>
+    <t>Stapler</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Test Product 2</t>
+  </si>
+  <si>
+    <t>AAA-5030544</t>
+  </si>
+  <si>
+    <t>MA-7383995</t>
+  </si>
+  <si>
+    <t>Large Spoon</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Test Product 3</t>
   </si>
 </sst>
 </file>
@@ -1004,19 +1034,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="19.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="9.57142857142857" customWidth="1"/>
+    <col min="3" max="3" width="12.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="12.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="14.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
@@ -1051,6 +1081,40 @@
       </c>
       <c r="E2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>